<commit_message>
Created progress tracker for the real numbers and real analysis
</commit_message>
<xml_diff>
--- a/Progress Tracker.xlsx
+++ b/Progress Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TeX\Books\Repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B298CA98-B94D-4414-A8F0-972789F339EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A23026-BD29-4862-B2FF-CC6108F8C67D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="887" xr2:uid="{0A31F4F4-7693-4728-9D2B-CBC85AC15615}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="887" activeTab="2" xr2:uid="{0A31F4F4-7693-4728-9D2B-CBC85AC15615}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1643,7 +1643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54C1F32-B421-4946-974E-A62B7E8038DC}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -4247,17 +4247,17 @@
     <row r="59" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -4340,8 +4340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45188445-E4C6-4C70-8A5D-19FE80CA1088}">
   <dimension ref="A1:V97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
@@ -19999,11 +19999,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="EC1:EJ1"/>
-    <mergeCell ref="EK1:EV1"/>
-    <mergeCell ref="EW1:FJ1"/>
-    <mergeCell ref="FK1:FW1"/>
-    <mergeCell ref="FX1:GD1"/>
     <mergeCell ref="DS1:EB1"/>
     <mergeCell ref="B1:K1"/>
     <mergeCell ref="L1:W1"/>
@@ -20016,6 +20011,11 @@
     <mergeCell ref="CJ1:CS1"/>
     <mergeCell ref="CT1:DC1"/>
     <mergeCell ref="DD1:DR1"/>
+    <mergeCell ref="EC1:EJ1"/>
+    <mergeCell ref="EK1:EV1"/>
+    <mergeCell ref="EW1:FJ1"/>
+    <mergeCell ref="FK1:FW1"/>
+    <mergeCell ref="FX1:GD1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -22888,12 +22888,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:T1"/>
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="X1:Z1"/>
     <mergeCell ref="BD1:BG1"/>
     <mergeCell ref="BH1:BK1"/>
     <mergeCell ref="BL1:BO1"/>
@@ -22904,6 +22898,12 @@
     <mergeCell ref="AQ1:AT1"/>
     <mergeCell ref="AU1:AW1"/>
     <mergeCell ref="AX1:BC1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:T1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="X1:Z1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -50976,38 +50976,6 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:P1"/>
-    <mergeCell ref="Q1:V1"/>
-    <mergeCell ref="W1:AB1"/>
-    <mergeCell ref="AC1:AL1"/>
-    <mergeCell ref="AM1:AT1"/>
-    <mergeCell ref="AU1:AZ1"/>
-    <mergeCell ref="BA1:BH1"/>
-    <mergeCell ref="BI1:BP1"/>
-    <mergeCell ref="EM1:ER1"/>
-    <mergeCell ref="ES1:EZ1"/>
-    <mergeCell ref="BQ1:BX1"/>
-    <mergeCell ref="BY1:CF1"/>
-    <mergeCell ref="CG1:CL1"/>
-    <mergeCell ref="CM1:CT1"/>
-    <mergeCell ref="CU1:DB1"/>
-    <mergeCell ref="DC1:DH1"/>
-    <mergeCell ref="DI1:DN1"/>
-    <mergeCell ref="DO1:DX1"/>
-    <mergeCell ref="DY1:EF1"/>
-    <mergeCell ref="EG1:EL1"/>
-    <mergeCell ref="JK1:JN1"/>
-    <mergeCell ref="JO1:JT1"/>
-    <mergeCell ref="JU1:JZ1"/>
-    <mergeCell ref="KA1:KD1"/>
-    <mergeCell ref="HS1:HZ1"/>
-    <mergeCell ref="IA1:IF1"/>
-    <mergeCell ref="IG1:IL1"/>
-    <mergeCell ref="IM1:IR1"/>
-    <mergeCell ref="IS1:IX1"/>
-    <mergeCell ref="IY1:JD1"/>
-    <mergeCell ref="JE1:JJ1"/>
     <mergeCell ref="HM1:HR1"/>
     <mergeCell ref="FA1:FF1"/>
     <mergeCell ref="FG1:FL1"/>
@@ -51020,6 +50988,38 @@
     <mergeCell ref="GW1:HB1"/>
     <mergeCell ref="HC1:HH1"/>
     <mergeCell ref="HI1:HL1"/>
+    <mergeCell ref="JK1:JN1"/>
+    <mergeCell ref="JO1:JT1"/>
+    <mergeCell ref="JU1:JZ1"/>
+    <mergeCell ref="KA1:KD1"/>
+    <mergeCell ref="HS1:HZ1"/>
+    <mergeCell ref="IA1:IF1"/>
+    <mergeCell ref="IG1:IL1"/>
+    <mergeCell ref="IM1:IR1"/>
+    <mergeCell ref="IS1:IX1"/>
+    <mergeCell ref="IY1:JD1"/>
+    <mergeCell ref="JE1:JJ1"/>
+    <mergeCell ref="ES1:EZ1"/>
+    <mergeCell ref="BQ1:BX1"/>
+    <mergeCell ref="BY1:CF1"/>
+    <mergeCell ref="CG1:CL1"/>
+    <mergeCell ref="CM1:CT1"/>
+    <mergeCell ref="CU1:DB1"/>
+    <mergeCell ref="DC1:DH1"/>
+    <mergeCell ref="DI1:DN1"/>
+    <mergeCell ref="DO1:DX1"/>
+    <mergeCell ref="DY1:EF1"/>
+    <mergeCell ref="EG1:EL1"/>
+    <mergeCell ref="AM1:AT1"/>
+    <mergeCell ref="AU1:AZ1"/>
+    <mergeCell ref="BA1:BH1"/>
+    <mergeCell ref="BI1:BP1"/>
+    <mergeCell ref="EM1:ER1"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I1:P1"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="W1:AB1"/>
+    <mergeCell ref="AC1:AL1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>